<commit_message>
modify the readme file
</commit_message>
<xml_diff>
--- a/diagnostics/emd/data/eddycurrent.xlsx
+++ b/diagnostics/emd/data/eddycurrent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375"/>
+    <workbookView windowWidth="18855" windowHeight="11235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="79">
   <si>
     <t>单独CS放电 （被动板是主要涡流来源）</t>
   </si>
@@ -380,6 +380,18 @@
   </si>
   <si>
     <t>滤波不一致，</t>
+  </si>
+  <si>
+    <t>1213-1215</t>
+  </si>
+  <si>
+    <t>165和345只装中间段，345切开，coil11测量1-6部分</t>
+  </si>
+  <si>
+    <t>COIL01套在限制器和磁通环后面</t>
+  </si>
+  <si>
+    <t>COIl07,COIL05 上下偏滤器、COIL03，COIL10上下被动板  COIL01 磁通环*7</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1119,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1150,22 +1162,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1696,10 +1699,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="30" customHeight="1"/>
@@ -2811,8 +2814,8 @@
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
     </row>
     <row r="43" customHeight="1" spans="1:12">
       <c r="A43" s="11" t="s">
@@ -2845,7 +2848,7 @@
       <c r="J43" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K43" s="18" t="s">
+      <c r="K43" s="16" t="s">
         <v>36</v>
       </c>
       <c r="L43" s="12" t="s">
@@ -2915,13 +2918,13 @@
       <c r="H45" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I45" s="18" t="s">
+      <c r="I45" s="16" t="s">
         <v>18</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K45" s="18" t="s">
+      <c r="K45" s="16" t="s">
         <v>39</v>
       </c>
       <c r="L45" s="12" t="s">
@@ -2977,101 +2980,101 @@
       <c r="A51" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D51" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="F51" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G51" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H51" s="14" t="s">
+      <c r="G51" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H51" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I51" s="14" t="s">
+      <c r="I51" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J51" s="14" t="s">
+      <c r="J51" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K51" s="19"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="19"/>
-      <c r="N51" s="19"/>
-      <c r="O51" s="19"/>
-      <c r="P51" s="19"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
     </row>
     <row r="52" customHeight="1" spans="1:10">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="16">
+      <c r="B52" s="5">
         <v>2.5</v>
       </c>
-      <c r="C52" s="16">
+      <c r="C52" s="5">
         <v>2.5</v>
       </c>
-      <c r="D52" s="16">
+      <c r="D52" s="5">
         <v>2.5</v>
       </c>
-      <c r="E52" s="16">
+      <c r="E52" s="5">
         <v>2.5</v>
       </c>
-      <c r="F52" s="16">
+      <c r="F52" s="5">
         <v>2.5</v>
       </c>
-      <c r="G52" s="16">
+      <c r="G52" s="5">
         <v>2.5</v>
       </c>
-      <c r="H52" s="16">
+      <c r="H52" s="5">
         <v>2.5</v>
       </c>
-      <c r="I52" s="16">
+      <c r="I52" s="5">
         <v>3.3</v>
       </c>
-      <c r="J52" s="16">
+      <c r="J52" s="5">
         <v>2.5</v>
       </c>
     </row>
     <row r="53" customHeight="1" spans="1:10">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="C53" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="E53" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F53" s="16" t="s">
+      <c r="F53" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G53" s="16" t="s">
+      <c r="G53" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H53" s="16" t="s">
+      <c r="H53" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I53" s="16" t="s">
+      <c r="I53" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J53" s="20" t="s">
+      <c r="J53" s="17" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3084,77 +3087,77 @@
       <c r="A56" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D56" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E56" s="14" t="s">
+      <c r="E56" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F56" s="14" t="s">
+      <c r="F56" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G56" s="14" t="s">
+      <c r="G56" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H56" s="14" t="s">
+      <c r="H56" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="57" customHeight="1" spans="1:8">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="16">
+      <c r="B57" s="5">
         <v>2.5</v>
       </c>
-      <c r="C57" s="16">
+      <c r="C57" s="5">
         <v>2.5</v>
       </c>
-      <c r="D57" s="16">
+      <c r="D57" s="5">
         <v>2.5</v>
       </c>
-      <c r="E57" s="16">
+      <c r="E57" s="5">
         <v>2.5</v>
       </c>
-      <c r="F57" s="16">
+      <c r="F57" s="5">
         <v>2.5</v>
       </c>
-      <c r="G57" s="16">
+      <c r="G57" s="5">
         <v>2.5</v>
       </c>
-      <c r="H57" s="16">
+      <c r="H57" s="5">
         <v>2.5</v>
       </c>
     </row>
     <row r="58" customHeight="1" spans="1:8">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E58" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F58" s="16" t="s">
+      <c r="F58" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G58" s="16" t="s">
+      <c r="G58" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H58" s="16" t="s">
+      <c r="H58" s="5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3194,7 +3197,7 @@
       <c r="A63" s="1">
         <v>1207</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -3206,8 +3209,32 @@
         <v>1209</v>
       </c>
     </row>
+    <row r="65" customHeight="1" spans="1:2">
+      <c r="A65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" customHeight="1" spans="1:2">
+      <c r="A66" s="1">
+        <v>1220</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="67" customHeight="1" spans="1:2">
+      <c r="A67" s="1">
+        <v>1221</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="21">
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="B9:J9"/>
@@ -3226,6 +3253,9 @@
     <mergeCell ref="B49:J49"/>
     <mergeCell ref="B50:J50"/>
     <mergeCell ref="B55:J55"/>
+    <mergeCell ref="B65:H65"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="B67:G67"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>